<commit_message>
change mail, new dates, update excel
</commit_message>
<xml_diff>
--- a/00_assets/data/BD-jornadas-202506.xlsx
+++ b/00_assets/data/BD-jornadas-202506.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28723"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28724"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{990C3402-50A3-4FB5-8700-14B02D5B1E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{217EBC39-8390-4CA1-AD96-6A5746142E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D1-geoinformatica" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="81">
   <si>
     <t>Comienzo</t>
   </si>
@@ -168,7 +168,7 @@
     <t>Reto relámpago</t>
   </si>
   <si>
-    <t>Opción 2: Open Foris: herramientas OpenSource para la gestión forestal</t>
+    <t>Opción 2: Open Foris: herramientas Open Source para la gestión forestal</t>
   </si>
   <si>
     <t>Pilar Valbuena</t>
@@ -264,7 +264,7 @@
     <t>Opción 1: Estadística aplicada a inventarios forestales</t>
   </si>
   <si>
-    <t>Opción 2: Conectividad de ecosistemas con machine learning</t>
+    <t>Opción 2: Calculo de conectividad de ecosistemas</t>
   </si>
   <si>
     <t>Carlos Rivas</t>
@@ -637,19 +637,26 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -659,13 +666,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1009,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1079,10 +1079,10 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="31">
+      <c r="A4" s="32">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="32">
         <v>0.47916666666666669</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1097,8 +1097,8 @@
       <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1127,10 +1127,10 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="31">
+      <c r="A7" s="32">
         <v>0.5</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="35">
         <v>0.5625</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1147,8 +1147,8 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="31"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
@@ -1163,8 +1163,8 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="31"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
@@ -1193,10 +1193,10 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="29">
+      <c r="A11" s="33">
         <v>0.60416666666666663</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="33">
         <v>0.61458333333333337</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -1211,8 +1211,8 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1225,10 +1225,10 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="29">
+      <c r="A13" s="33">
         <v>0.61458333333333337</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="33">
         <v>0.625</v>
       </c>
       <c r="C13" s="23" t="s">
@@ -1243,8 +1243,8 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
@@ -1257,10 +1257,10 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="31">
+      <c r="A15" s="32">
         <v>0.625</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="32">
         <v>0.6875</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1275,8 +1275,8 @@
       <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
@@ -1291,8 +1291,8 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="7" t="s">
         <v>36</v>
       </c>
@@ -1323,10 +1323,10 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="29">
+      <c r="A19" s="33">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="33">
         <v>0.77083333333333337</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="7" t="s">
         <v>38</v>
       </c>
@@ -1359,8 +1359,8 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="7" t="s">
         <v>39</v>
       </c>
@@ -1375,10 +1375,10 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="38">
+      <c r="A22" s="30">
         <v>0.85416666666666663</v>
       </c>
-      <c r="B22" s="39">
+      <c r="B22" s="31">
         <v>0.95833333333333337</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1396,18 +1396,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1419,7 +1419,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1471,10 +1471,10 @@
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="29">
+      <c r="A3" s="33">
         <v>0.375</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="33">
         <v>0.45833333333333331</v>
       </c>
       <c r="C3" s="28" t="s">
@@ -1489,8 +1489,8 @@
       <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="7" t="s">
         <v>45</v>
       </c>
@@ -1521,10 +1521,10 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="33">
+      <c r="A6" s="35">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="35">
         <v>0.5625</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1539,8 +1539,8 @@
       <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="7" t="s">
         <v>48</v>
       </c>
@@ -1550,11 +1550,13 @@
       <c r="E7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="26" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="7" t="s">
         <v>49</v>
       </c>
@@ -1583,10 +1585,10 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="33">
+      <c r="A10" s="35">
         <v>0.60416666666666663</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="35">
         <v>0.61458333333333337</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1601,8 +1603,8 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="7" t="s">
         <v>53</v>
       </c>
@@ -1615,10 +1617,10 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="33">
+      <c r="A12" s="35">
         <v>0.61458333333333337</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="35">
         <v>0.625</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -1633,8 +1635,8 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="7" t="s">
         <v>56</v>
       </c>
@@ -1647,10 +1649,10 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="33">
+      <c r="A14" s="35">
         <v>0.625</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="35">
         <v>0.6875</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1667,8 +1669,8 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="7" t="s">
         <v>58</v>
       </c>
@@ -1683,8 +1685,8 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="7" t="s">
         <v>61</v>
       </c>
@@ -1715,10 +1717,10 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="29">
+      <c r="A18" s="33">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="33">
         <v>0.77083333333333337</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1730,11 +1732,13 @@
       <c r="E18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="26"/>
+      <c r="F18" s="28" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="7" t="s">
         <v>63</v>
       </c>
@@ -1749,8 +1753,8 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="7" t="s">
         <v>65</v>
       </c>
@@ -1804,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07A4528-549F-4881-AF93-621EB587BE44}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1858,10 +1862,10 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="34">
+      <c r="A3" s="37">
         <v>0.375</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="37">
         <v>0.38541666666666669</v>
       </c>
       <c r="C3" s="20" t="s">
@@ -1878,8 +1882,8 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="20" t="s">
         <v>70</v>
       </c>
@@ -1894,10 +1898,10 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="34">
+      <c r="A5" s="37">
         <v>0.38541666666666669</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="37">
         <v>0.39583333333333331</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -1914,8 +1918,8 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="20" t="s">
         <v>72</v>
       </c>
@@ -1930,10 +1934,10 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="34">
+      <c r="A7" s="37">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="37">
         <v>0.45833333333333331</v>
       </c>
       <c r="C7" s="20" t="s">
@@ -1950,8 +1954,8 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="20" t="s">
         <v>74</v>
       </c>
@@ -1966,8 +1970,8 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="20" t="s">
         <v>76</v>
       </c>
@@ -2002,10 +2006,10 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="34">
+      <c r="A11" s="37">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="37">
         <v>0.57291666666666663</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -2022,8 +2026,8 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="20" t="s">
         <v>78</v>
       </c>
@@ -2038,8 +2042,8 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="20" t="s">
         <v>79</v>
       </c>
@@ -2069,7 +2073,7 @@
       <c r="E14" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="29" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove renv, add pablo, edit calendar
</commit_message>
<xml_diff>
--- a/00_assets/data/BD-jornadas-202506.xlsx
+++ b/00_assets/data/BD-jornadas-202506.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29012"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{962C1AF4-5BAF-4903-964E-49A3515A1B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3674A32-68EF-4896-898E-5FBDAEFE5986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D1-geoinformatica" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
     <t>Ayudante</t>
   </si>
   <si>
-    <t>Apertura + Bosque digital + Máster geoforest</t>
+    <t>Aula 1: Apertura + Bosque digital + Máster geoforest</t>
   </si>
   <si>
     <t>Charla</t>
@@ -117,10 +117,10 @@
     <t>Rafael Navarro</t>
   </si>
   <si>
-    <t>Estado del arte de la geomática y la teledetección (nuevos sensores, tendencias...)</t>
-  </si>
-  <si>
-    <t>Opción 1: Introducción a SIG con QGIS</t>
+    <t>Aula 1: Estado del arte de la geomática y la teledetección (nuevos sensores, tendencias...)</t>
+  </si>
+  <si>
+    <t>Aula 1: Introducción a SIG con QGIS</t>
   </si>
   <si>
     <t>Workshop</t>
@@ -129,7 +129,7 @@
     <t>Fran Ruiz</t>
   </si>
   <si>
-    <t>Opción 2: Model builder de QGIS</t>
+    <t>Aula 2: Model builder de QGIS</t>
   </si>
   <si>
     <t>Carlos Martín</t>
@@ -141,19 +141,19 @@
     <t>Descanso</t>
   </si>
   <si>
-    <t>Opción 1: Introducción al análisis de datos con R</t>
+    <t>Aula 1: Introducción al análisis de datos con R</t>
   </si>
   <si>
     <t>Pablo González</t>
   </si>
   <si>
-    <t>Opción 2: Introducción a la programación con Python</t>
+    <t>Aula 2: Introducción a la programación con Python</t>
   </si>
   <si>
     <t>Mauricio</t>
   </si>
   <si>
-    <t>Opción 3: Introducción a bases de datos y SQL</t>
+    <t>Aula 3: Introducción a bases de datos y SQL</t>
   </si>
   <si>
     <t>Mari Ángeles</t>
@@ -162,34 +162,34 @@
     <t>Comida</t>
   </si>
   <si>
-    <t>Opción 1: Ordenación de montes: del inventario a la selvicultura</t>
+    <t>Aula 1: Ordenación de montes: del inventario a la selvicultura</t>
   </si>
   <si>
     <t>Reto relámpago</t>
   </si>
   <si>
-    <t>Opción 2: Open Foris: herramientas Open Source para la gestión forestal</t>
+    <t>Aula 2: Open Foris: herramientas Open Source para la gestión forestal</t>
   </si>
   <si>
     <t>Pilar Valbuena</t>
   </si>
   <si>
-    <t>Opción 1: Impacto del cambio climático</t>
+    <t>Aula 1: Impacto del cambio climático</t>
   </si>
   <si>
     <t>Guillermo Palacios</t>
   </si>
   <si>
-    <t>Opción 2: Positron - Una IDE para ciencia de datos con R y Python</t>
+    <t>Aula 2: Positron - Una IDE para ciencia de datos con R y Python</t>
   </si>
   <si>
     <t>Adrián Cidre</t>
   </si>
   <si>
-    <t>Opción 1: Introducción a análisis geoespacial con R</t>
-  </si>
-  <si>
-    <t>Opción 2: Análisis de datos con GEE</t>
+    <t>Aula 1: Introducción a análisis geoespacial con R</t>
+  </si>
+  <si>
+    <t>Aula 2: Análisis de datos con GEE</t>
   </si>
   <si>
     <t>Antonio J. Molina</t>
@@ -198,16 +198,16 @@
     <t>Javier Pérez</t>
   </si>
   <si>
-    <t>Opción 3: Introducción a programación lineal</t>
-  </si>
-  <si>
-    <t>Opcón 1: Introducción 2 a análisis geoespacial con R</t>
-  </si>
-  <si>
-    <t>Opción 2: Análisis 2 de datos con Google Earth Engine</t>
-  </si>
-  <si>
-    <t>Opción 3: Introducción 2 a programación lineal</t>
+    <t>Aula 3: Introducción a programación lineal</t>
+  </si>
+  <si>
+    <t>Aula 1: Introducción 2 a análisis geoespacial con R</t>
+  </si>
+  <si>
+    <t>Aula 2: Análisis 2 de datos con Google Earth Engine</t>
+  </si>
+  <si>
+    <t>Aula 3: Introducción 2 a programación lineal</t>
   </si>
   <si>
     <t>Mauricio Acuña</t>
@@ -219,118 +219,118 @@
     <t>Cervezas con ciencia (espacio abierto festivo de geociencias forestales)</t>
   </si>
   <si>
-    <t>Machine Learning e IA en ciencias forestales</t>
-  </si>
-  <si>
-    <t>Opción 1: Tecnología FAO para toma de datos de campo: uso de Arena y Ground</t>
-  </si>
-  <si>
-    <t>Opción 2: Descarga de datos y teledetección con R (descarga, exploración, IVeg ...)</t>
+    <t>Aula 1: Machine Learning e IA en ciencias forestales</t>
+  </si>
+  <si>
+    <t>Aula 1: Tecnología FAO para toma de datos de campo: uso de Arena y Ground</t>
+  </si>
+  <si>
+    <t>Aula 2: Descarga de datos y teledetección con R (descarga, exploración, IVeg ...)</t>
   </si>
   <si>
     <t>Antonio Ariza?</t>
   </si>
   <si>
-    <t>Opción 1: Clasificación de usos del suelo en R (GEOBIA)</t>
-  </si>
-  <si>
-    <t>Opción 2: Clasificación de usos del suelo con GEE</t>
-  </si>
-  <si>
-    <t>Opción 3: Desarrollo de modelos alométricos para biomasa</t>
+    <t>Aula 1: Clasificación de usos del suelo en R (GEOBIA)</t>
+  </si>
+  <si>
+    <t>Aula 2: Clasificación de usos del suelo con GEE</t>
+  </si>
+  <si>
+    <t>Aula 3: Modelos de Distribución de Especies: conceptos y aplicación</t>
+  </si>
+  <si>
+    <t>Ricardo Hernández</t>
+  </si>
+  <si>
+    <t>Pablo Gonzalez</t>
+  </si>
+  <si>
+    <t>Aula 1: Teledetección y gestión de bosques australes</t>
+  </si>
+  <si>
+    <t>Antonio Cabrera</t>
+  </si>
+  <si>
+    <t>Aula 2: Paralelización en R</t>
+  </si>
+  <si>
+    <t>Opcion 1: Idoneidad del Hábitat vía SDMs y Decaimiento Forestal</t>
+  </si>
+  <si>
+    <t>Aula 2: Potencialides de SAGA GIS  para análisis hidrológicos y de erosión</t>
+  </si>
+  <si>
+    <t>Aula 1: Estadística aplicada a inventarios forestales</t>
+  </si>
+  <si>
+    <t>Aula 2: Calculo de conectividad de ecosistemas</t>
+  </si>
+  <si>
+    <t>Carlos Rivas</t>
+  </si>
+  <si>
+    <t>Guillermo</t>
+  </si>
+  <si>
+    <t>Aula 3: Intermedio - Optimización 1</t>
+  </si>
+  <si>
+    <t>Aula 1: Estadística aplicada a inventarios forestales 2</t>
+  </si>
+  <si>
+    <t>Aula 2: Desarrollo de modelos alométricos para biomasa</t>
   </si>
   <si>
     <t>Antonio Ariza</t>
   </si>
   <si>
-    <t>Opción 1: Teledetección y gestión de bosques australes</t>
-  </si>
-  <si>
-    <t>Antonio Cabrera</t>
-  </si>
-  <si>
-    <t>Opción 2: Paralelización en R</t>
-  </si>
-  <si>
-    <t>Opcion 1: Modelos de nicho y áreas protegidas</t>
-  </si>
-  <si>
-    <t>Ricardo Hernández</t>
-  </si>
-  <si>
-    <t>Opción 2: Potencialides de SAGA GIS  para análisis hidrológicos y de erosión</t>
-  </si>
-  <si>
-    <t>Opción 1: Estadística aplicada a inventarios forestales</t>
-  </si>
-  <si>
-    <t>Opción 2: Calculo de conectividad de ecosistemas</t>
-  </si>
-  <si>
-    <t>Carlos Rivas</t>
-  </si>
-  <si>
-    <t>Guillermo</t>
-  </si>
-  <si>
-    <t>Opción 3: Intermedio - Optimización 1</t>
-  </si>
-  <si>
-    <t>Opción 1: Estadística aplicada a inventarios forestales 2</t>
-  </si>
-  <si>
-    <t>Opción 2: Modelos predictivos aplicados a la priorización sistemática de la conservación</t>
-  </si>
-  <si>
-    <t>Pablo Gonzalez</t>
-  </si>
-  <si>
-    <t>Opción 3: Intermedio - Optimización 2</t>
-  </si>
-  <si>
-    <t>Estado del arte de los sensores close remote sensing</t>
+    <t>Aula 3: Intermedio - Optimización 2</t>
+  </si>
+  <si>
+    <t>Aula 1: Estado del arte de los sensores close remote sensing</t>
   </si>
   <si>
     <t>Rafa Navarro</t>
   </si>
   <si>
-    <t>Opción 1: Ecofisiología y sensorización del decaimiento forestal</t>
+    <t>Aula 1: Ecofisiología y sensorización del decaimiento forestal</t>
   </si>
   <si>
     <t> </t>
   </si>
   <si>
-    <t>Opción 2: Incendios forestales</t>
-  </si>
-  <si>
-    <t>Opción 1: Fragmentación forestal: conceptos y métricas</t>
-  </si>
-  <si>
-    <t>Opción 2: Sensorización LiDAR de procesadoras forestales</t>
-  </si>
-  <si>
-    <t>Opción 1: Toma de datos fotogramétricos + exploración de datos</t>
-  </si>
-  <si>
-    <t>Opción 2: Preprocesado de datos LiDAR + obtención de modelos digitales y métricas con lidR</t>
+    <t>Aula 2: Incendios forestales</t>
+  </si>
+  <si>
+    <t>Aula 1: Fragmentación forestal: conceptos y métricas</t>
+  </si>
+  <si>
+    <t>Aula 2: Sensorización LiDAR de procesadoras forestales</t>
+  </si>
+  <si>
+    <t>Aula 1: Toma de datos fotogramétricos + exploración de datos</t>
+  </si>
+  <si>
+    <t>Aula 2: Preprocesado de datos LiDAR + obtención de modelos digitales y métricas con lidR</t>
   </si>
   <si>
     <t>Mª Ángeles</t>
   </si>
   <si>
-    <t>Opción 3: Procesado de nubes de puntos con Python</t>
-  </si>
-  <si>
-    <t>Opción 1: LiDAR para inventario forestal con lidR</t>
-  </si>
-  <si>
-    <t>Opción 2: Procesado de datos de TLS para inventario forestal</t>
-  </si>
-  <si>
-    <t>Opción 3: Análisis de árbol individual</t>
-  </si>
-  <si>
-    <t>Cierre Summer School</t>
+    <t>Aula 3: Procesado de nubes de puntos con Python</t>
+  </si>
+  <si>
+    <t>Aula 1: LiDAR para inventario forestal con lidR</t>
+  </si>
+  <si>
+    <t>Aula 2: Procesado de datos de TLS para inventario forestal</t>
+  </si>
+  <si>
+    <t>Aula 3: Análisis de árbol individual</t>
+  </si>
+  <si>
+    <t>Aula 1: Cierre Summer School</t>
   </si>
 </sst>
 </file>
@@ -644,19 +644,19 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1010,7 +1010,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1079,10 +1079,10 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="32">
+      <c r="A4" s="34">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="34">
         <v>0.47916666666666669</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1097,8 +1097,8 @@
       <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1127,10 +1127,10 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="32">
+      <c r="A7" s="34">
         <v>0.5</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="36">
         <v>0.5625</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1147,8 +1147,8 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="32"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
@@ -1163,8 +1163,8 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="32"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
@@ -1193,10 +1193,10 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="33">
+      <c r="A11" s="32">
         <v>0.60416666666666663</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="32">
         <v>0.61458333333333337</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -1211,8 +1211,8 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1225,10 +1225,10 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="33">
+      <c r="A13" s="32">
         <v>0.61458333333333337</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>0.625</v>
       </c>
       <c r="C13" s="23" t="s">
@@ -1243,8 +1243,8 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
@@ -1257,10 +1257,10 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="32">
+      <c r="A15" s="34">
         <v>0.625</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="34">
         <v>0.6875</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1275,8 +1275,8 @@
       <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
@@ -1291,8 +1291,8 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="7" t="s">
         <v>36</v>
       </c>
@@ -1323,10 +1323,10 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="33">
+      <c r="A19" s="32">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="32">
         <v>0.77083333333333337</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="7" t="s">
         <v>38</v>
       </c>
@@ -1359,8 +1359,8 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="7" t="s">
         <v>39</v>
       </c>
@@ -1396,18 +1396,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1419,7 +1419,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1471,10 +1471,10 @@
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="33">
+      <c r="A3" s="32">
         <v>0.375</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="32">
         <v>0.45833333333333331</v>
       </c>
       <c r="C3" s="28" t="s">
@@ -1489,8 +1489,8 @@
       <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>45</v>
       </c>
@@ -1521,10 +1521,10 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="35">
+      <c r="A6" s="36">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="36">
         <v>0.5625</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1539,8 +1539,8 @@
       <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="7" t="s">
         <v>48</v>
       </c>
@@ -1550,13 +1550,13 @@
       <c r="E7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="7" t="s">
         <v>49</v>
       </c>
@@ -1566,7 +1566,9 @@
       <c r="E8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="26"/>
+      <c r="F8" s="28" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="6">
@@ -1585,28 +1587,28 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="35">
+      <c r="A10" s="36">
         <v>0.60416666666666663</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="36">
         <v>0.61458333333333337</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>25</v>
@@ -1617,26 +1619,26 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="35">
+      <c r="A12" s="36">
         <v>0.61458333333333337</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="36">
         <v>0.625</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="7" t="s">
         <v>56</v>
       </c>
@@ -1649,10 +1651,10 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="35">
+      <c r="A14" s="36">
         <v>0.625</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="36">
         <v>0.6875</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1669,8 +1671,8 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="7" t="s">
         <v>58</v>
       </c>
@@ -1685,8 +1687,8 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="7" t="s">
         <v>61</v>
       </c>
@@ -1717,10 +1719,10 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="33">
+      <c r="A18" s="32">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="32">
         <v>0.77083333333333337</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1737,8 +1739,8 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="7" t="s">
         <v>63</v>
       </c>
@@ -1746,15 +1748,13 @@
         <v>11</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="28" t="s">
         <v>64</v>
       </c>
+      <c r="F19" s="26"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="7" t="s">
         <v>65</v>
       </c>
@@ -1809,7 +1809,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1963,7 +1963,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>75</v>
@@ -2022,7 +2022,7 @@
         <v>75</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2035,7 +2035,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="F12" s="27" t="s">
         <v>69</v>

</xml_diff>